<commit_message>
Finalized things, made visual improvements.
</commit_message>
<xml_diff>
--- a/YearbookVerify/Final Package/input.xlsx
+++ b/YearbookVerify/Final Package/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="27795" windowHeight="11820"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>First Name</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Input Here \/</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Smith</t>
   </si>
 </sst>
 </file>
@@ -385,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C4"/>
+  <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,6 +434,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>

</xml_diff>